<commit_message>
Fix minor errors on map
</commit_message>
<xml_diff>
--- a/Data/correct_farm_names.xlsx
+++ b/Data/correct_farm_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\starr\Google Drive\Career Projects\Projects\Harvest Against Hunger Summer '21\harvest-against-hunger\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF62BDB-73B4-4AB1-A19D-93EAEC115948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA7878B-76C6-43B4-B387-E693EE6F82F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="107">
   <si>
     <t>Farm Name</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>Ecolibrium Farm</t>
+  </si>
+  <si>
+    <t>Farmstand Local Foods (distributor)</t>
   </si>
 </sst>
 </file>
@@ -730,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +939,7 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -944,7 +947,7 @@
         <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1520,7 +1523,7 @@
         <v>66</v>
       </c>
       <c r="B98" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>